<commit_message>
write the report and debugs
</commit_message>
<xml_diff>
--- a/question2/result.xlsx
+++ b/question2/result.xlsx
@@ -14,138 +14,141 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Date Eliminated</t>
+  </si>
+  <si>
+    <t>Memphis Grizzlies</t>
+  </si>
+  <si>
+    <t>Playoff</t>
+  </si>
+  <si>
+    <t>Dallas Mavericks</t>
+  </si>
+  <si>
+    <t>03/27/2017</t>
+  </si>
+  <si>
+    <t>Milwaukee Bucks</t>
+  </si>
+  <si>
+    <t>Los Angeles Lakers</t>
+  </si>
+  <si>
+    <t>03/12/2017</t>
+  </si>
+  <si>
+    <t>New York Knicks</t>
+  </si>
+  <si>
+    <t>03/22/2017</t>
+  </si>
+  <si>
+    <t>Phoenix Suns</t>
+  </si>
+  <si>
+    <t>New Orleans Pelicans</t>
+  </si>
+  <si>
+    <t>03/30/2017</t>
+  </si>
+  <si>
+    <t>Oklahoma City Thunder</t>
+  </si>
+  <si>
+    <t>Houston Rockets</t>
+  </si>
+  <si>
+    <t>Boston Celtics</t>
+  </si>
+  <si>
+    <t>Philadelphia 76ers</t>
+  </si>
+  <si>
+    <t>Charlotte Hornets</t>
+  </si>
+  <si>
+    <t>04/06/2017</t>
+  </si>
+  <si>
+    <t>Miami Heat</t>
+  </si>
+  <si>
+    <t>04/12/2017</t>
+  </si>
+  <si>
+    <t>Denver Nuggets</t>
+  </si>
+  <si>
+    <t>04/08/2017</t>
+  </si>
+  <si>
+    <t>San Antonio Spurs</t>
+  </si>
+  <si>
+    <t>Brooklyn Nets</t>
+  </si>
+  <si>
+    <t>02/15/2017</t>
+  </si>
+  <si>
+    <t>Minnesota Timberwolves</t>
+  </si>
+  <si>
+    <t>03/24/2017</t>
+  </si>
+  <si>
+    <t>Atlanta Hawks</t>
+  </si>
+  <si>
+    <t>Cleveland Cavaliers</t>
+  </si>
+  <si>
+    <t>Indiana Pacers</t>
+  </si>
+  <si>
+    <t>Orlando Magic</t>
+  </si>
+  <si>
+    <t>03/16/2017</t>
+  </si>
+  <si>
+    <t>LA Clippers</t>
+  </si>
+  <si>
+    <t>Sacramento Kings</t>
+  </si>
+  <si>
+    <t>03/19/2017</t>
+  </si>
+  <si>
+    <t>Portland Trail Blazers</t>
+  </si>
+  <si>
+    <t>Golden State Warriors</t>
+  </si>
   <si>
     <t>Chicago Bulls</t>
   </si>
   <si>
-    <t>Playoff</t>
-  </si>
-  <si>
-    <t>Cleveland Cavaliers</t>
-  </si>
-  <si>
-    <t>Sacramento Kings</t>
-  </si>
-  <si>
-    <t>03/10/2017</t>
-  </si>
-  <si>
-    <t>Miami Heat</t>
-  </si>
-  <si>
-    <t>04/08/2017</t>
-  </si>
-  <si>
-    <t>New York Knicks</t>
-  </si>
-  <si>
-    <t>03/12/2017</t>
-  </si>
-  <si>
-    <t>Los Angeles Lakers</t>
-  </si>
-  <si>
-    <t>02/26/2017</t>
-  </si>
-  <si>
-    <t>Minnesota Timberwolves</t>
-  </si>
-  <si>
-    <t>03/19/2017</t>
-  </si>
-  <si>
-    <t>Golden State Warriors</t>
-  </si>
-  <si>
-    <t>Milwaukee Bucks</t>
-  </si>
-  <si>
-    <t>Memphis Grizzlies</t>
-  </si>
-  <si>
-    <t>Brooklyn Nets</t>
-  </si>
-  <si>
-    <t>01/28/2017</t>
-  </si>
-  <si>
     <t>Utah Jazz</t>
   </si>
   <si>
     <t>Washington Wizards</t>
   </si>
   <si>
-    <t>Atlanta Hawks</t>
-  </si>
-  <si>
-    <t>San Antonio Spurs</t>
-  </si>
-  <si>
-    <t>New Orleans Pelicans</t>
-  </si>
-  <si>
-    <t>03/30/2017</t>
-  </si>
-  <si>
     <t>Toronto Raptors</t>
   </si>
   <si>
-    <t>Dallas Mavericks</t>
-  </si>
-  <si>
-    <t>03/29/2017</t>
-  </si>
-  <si>
-    <t>Denver Nuggets</t>
-  </si>
-  <si>
-    <t>Orlando Magic</t>
-  </si>
-  <si>
-    <t>02/23/2017</t>
-  </si>
-  <si>
-    <t>Phoenix Suns</t>
-  </si>
-  <si>
-    <t>02/06/2017</t>
-  </si>
-  <si>
-    <t>Oklahoma City Thunder</t>
-  </si>
-  <si>
-    <t>Indiana Pacers</t>
-  </si>
-  <si>
-    <t>Houston Rockets</t>
-  </si>
-  <si>
-    <t>LA Clippers</t>
-  </si>
-  <si>
-    <t>Philadelphia 76ers</t>
-  </si>
-  <si>
-    <t>03/11/2017</t>
-  </si>
-  <si>
-    <t>Boston Celtics</t>
-  </si>
-  <si>
-    <t>Portland Trail Blazers</t>
-  </si>
-  <si>
     <t>Detroit Pistons</t>
   </si>
   <si>
     <t>04/05/2017</t>
-  </si>
-  <si>
-    <t>Charlotte Hornets</t>
-  </si>
-  <si>
-    <t>04/06/2017</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,7 +497,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -503,23 +506,23 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -543,15 +546,15 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -559,7 +562,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -567,7 +570,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -575,23 +578,23 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -599,63 +602,63 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -663,63 +666,63 @@
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -727,7 +730,15 @@
         <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
         <v>43</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>